<commit_message>
Cleaned rates in fix_delete and fix_nucleate
Removed ki factor as in Shvab, using pure TST. User must now input cx and dim in ChemDB.dat.
</commit_message>
<xml_diff>
--- a/tests/basic_Ca(OH)2-CaCO3/prepare_inputs.xlsx
+++ b/tests/basic_Ca(OH)2-CaCO3/prepare_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emasoero/GitHub/201224-MASKE_only/MASKE/tests/basic_Ca(OH)2-CaCO3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B51EC10-0D97-5C41-BD88-BA531D7F7E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D174D95-48E3-554A-A7F2-B0625D12CE77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="940" windowWidth="14880" windowHeight="12360" xr2:uid="{E5490447-C7E3-7F4E-8C18-F3CA77CAB1DC}"/>
+    <workbookView xWindow="920" yWindow="2240" windowWidth="16120" windowHeight="13720" xr2:uid="{E5490447-C7E3-7F4E-8C18-F3CA77CAB1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,11 +31,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>cm3/mol</t>
   </si>
   <si>
+    <t>nm3/molecule</t>
+  </si>
+  <si>
     <t>SOLID MOLECULE SIZE (CUBIC)</t>
   </si>
   <si>
@@ -129,17 +132,134 @@
     <t>PHREEQC W</t>
   </si>
   <si>
-    <t>apparet vol</t>
-  </si>
-  <si>
-    <t>nm^3, at infinite dilution (no Debye Huckel correction)</t>
+    <t>cm3/mol, at infinite dilution (no Debye Huckel correction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apparent vol </t>
+  </si>
+  <si>
+    <t>Ca+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SETS OF USEFUL PARAMETERS </t>
+  </si>
+  <si>
+    <t>OH-</t>
+  </si>
+  <si>
+    <t>CO3-2</t>
+  </si>
+  <si>
+    <t>mmol s-1 cm-2</t>
+  </si>
+  <si>
+    <t>mmol s-1 cm-2 L-1</t>
+  </si>
+  <si>
+    <t>kT/h</t>
+  </si>
+  <si>
+    <t>kT</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Js</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>s-1</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>ln(kh/kT)</t>
+  </si>
+  <si>
+    <t>with c* = 1 mmol/cm2</t>
+  </si>
+  <si>
+    <t>DS++</t>
+  </si>
+  <si>
+    <t>kB</t>
+  </si>
+  <si>
+    <t>KJ/mol/K</t>
+  </si>
+  <si>
+    <t>in KJ/mol/K with c* = 1 mol/cm2</t>
+  </si>
+  <si>
+    <t>TDS++</t>
+  </si>
+  <si>
+    <t>kJ/mol with c* = 1 mmol/cm2</t>
+  </si>
+  <si>
+    <t>in KJ/mol/K with c* = 1 mmol/cm2</t>
+  </si>
+  <si>
+    <t>mol/s/cm2</t>
+  </si>
+  <si>
+    <t>with c*=1 mol/cm2</t>
+  </si>
+  <si>
+    <t>kJ/mol with c* = 1 mol/cm2</t>
+  </si>
+  <si>
+    <t>s-1 cm-2</t>
+  </si>
+  <si>
+    <t>with c* in cm-2</t>
+  </si>
+  <si>
+    <t>in KJ/mol/K with c* = 1 cm-2</t>
+  </si>
+  <si>
+    <t>in KJ/mol with c* = 1 cm-2</t>
+  </si>
+  <si>
+    <t>s-1 nm-2</t>
+  </si>
+  <si>
+    <t>with c* in nm-2</t>
+  </si>
+  <si>
+    <t>in KJ/mol/K with c* = 1 nm-2</t>
+  </si>
+  <si>
+    <t>in KJ/mol with c* = 1 nm-2</t>
+  </si>
+  <si>
+    <t>CALCULATION OF DS++ FOR CAOH from JOHANSSEN: TO BE WRITTEN DOWN PROPERLY…</t>
+  </si>
+  <si>
+    <t>CAOH2 = Ca + 2H2O - 2H</t>
+  </si>
+  <si>
+    <t>H2O = OH + H</t>
+  </si>
+  <si>
+    <t>CaOH2 = Ca + 2OH</t>
+  </si>
+  <si>
+    <t>log K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +276,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -201,13 +329,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,65 +652,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC077A22-B44D-AA4B-965B-7E1EF36C7611}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:14">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3">
         <v>100.0869</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="3">
-        <v>-0.34560000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
         <v>2.71</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3">
-        <v>-7.2519999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <f>C3/C4</f>
@@ -590,163 +720,587 @@
         <v>0</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3">
-        <v>6.149</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <f>C5/6.022E+23*1E+21</f>
         <v>6.1329185360933652E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="3">
-        <v>-2.4790000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
+        <v>-5.67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <f>C6^(1/3)</f>
         <v>0.39435655613657195</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3">
-        <v>1.2390000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
+        <v>6.85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3">
         <v>1.01325</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="3">
         <v>298</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
       <c r="F10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3">
         <v>78.400000000000006</v>
       </c>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
       <c r="F11" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
       <c r="F12" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" s="5">
         <f>G3*0.1</f>
-        <v>-3.456E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
+        <v>0.59500000000000008</v>
+      </c>
+      <c r="M12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12">
+        <v>22.799937</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5">
         <f>G4*100/(2600+G8)</f>
-        <v>-0.27881441972661997</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5">
         <f>G5/(G9-228)</f>
-        <v>8.7842857142857139E-2</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
       <c r="F15" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G15" s="5">
         <f>G6*10000/((2600+G8)*(G9-228))</f>
-        <v>-0.13615572974988005</v>
-      </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
+        <v>-0.31141709870182321</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
       <c r="F16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="5">
         <f>1/G10/G10*G11</f>
         <v>9.7615576842982065E-7</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16">
+        <f>N12+N14+N14</f>
+        <v>-5.2000630000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14">
       <c r="F17" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" s="5">
         <f>G7*G16</f>
-        <v>1.2094569970845479E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8">
+        <v>6.6866670137442713E-6</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17">
+        <f>10^N16</f>
+        <v>6.3086582264109297E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14">
       <c r="F18" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G18" s="5">
-        <f>41.84*(G12+G13+G14+G15-G17)/1000</f>
-        <v>-1.5133046914920376E-2</v>
+        <f>41.84*(G12+G13+G14+G15-G17)</f>
+        <v>11.864828820167865</v>
       </c>
       <c r="H18" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="19" spans="6:14">
+      <c r="F19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="5">
+        <f>G18/6.022E+23*1E+21</f>
+        <v>1.9702472301839694E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14">
+      <c r="F22" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14">
+      <c r="F23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14">
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="3">
+        <v>-0.34560000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="6:14">
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="3">
+        <v>-7.2519999999999998</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="6:14">
+      <c r="F26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="3">
+        <v>6.149</v>
+      </c>
+    </row>
+    <row r="27" spans="6:14">
+      <c r="F27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="3">
+        <v>-2.4790000000000001</v>
+      </c>
+      <c r="J27" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27">
+        <f>EXP(-10)</f>
+        <v>4.5399929762484854E-5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="6:14">
+      <c r="F28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1.2390000000000001</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
+      <c r="K28">
+        <f>K27*0.75</f>
+        <v>3.4049947321863639E-5</v>
+      </c>
+      <c r="L28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="6:14">
+      <c r="J29" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="7">
+        <v>4.1099999999999998E-21</v>
+      </c>
+      <c r="L29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="6:14">
+      <c r="F30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30">
+        <f>6.626E-34</f>
+        <v>6.6259999999999998E-34</v>
+      </c>
+      <c r="L30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="6:14">
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="3">
+        <v>-9.66</v>
+      </c>
+      <c r="J31" t="s">
+        <v>41</v>
+      </c>
+      <c r="K31" s="7">
+        <f>K29/K30</f>
+        <v>6202837307576.2148</v>
+      </c>
+      <c r="L31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="6:14">
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="3">
+        <v>28.5</v>
+      </c>
+      <c r="J32" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="7">
+        <f>LN(K28/K31)</f>
+        <v>-39.743710006004811</v>
+      </c>
+      <c r="L32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12">
+      <c r="F33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="3">
+        <v>80</v>
+      </c>
+      <c r="J33" t="s">
+        <v>51</v>
+      </c>
+      <c r="K33">
+        <f>0.008314</f>
+        <v>8.3140000000000002E-3</v>
+      </c>
+      <c r="L33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12">
+      <c r="F34" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="3">
+        <v>-22.9</v>
+      </c>
+      <c r="J34" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="7">
+        <f>K33*K32</f>
+        <v>-0.33042920498992401</v>
+      </c>
+      <c r="L34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12">
+      <c r="F35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.89</v>
+      </c>
+      <c r="J35" t="s">
+        <v>54</v>
+      </c>
+      <c r="K35" s="7">
+        <f>K34*298</f>
+        <v>-98.467903086997353</v>
+      </c>
+      <c r="L35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12">
+      <c r="F37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37">
+        <f>K28/1000000</f>
+        <v>3.4049947321863637E-11</v>
+      </c>
+      <c r="L37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12">
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="3">
+        <v>5.95</v>
+      </c>
+      <c r="J38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38">
+        <f>LN(K37/K31)</f>
+        <v>-53.559220563969085</v>
+      </c>
+      <c r="L38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12">
+      <c r="F39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39">
+        <f>K38*K33</f>
+        <v>-0.44529135976883899</v>
+      </c>
+      <c r="L39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12">
+      <c r="F40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40">
+        <f>K39*298</f>
+        <v>-132.69682521111403</v>
+      </c>
+      <c r="L40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12">
+      <c r="F41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="3">
+        <v>-5.67</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12">
+      <c r="F42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="3">
+        <v>6.85</v>
+      </c>
+      <c r="J42" t="s">
+        <v>47</v>
+      </c>
+      <c r="K42">
+        <f>K37*6.022E+23</f>
+        <v>20504878277226.285</v>
+      </c>
+      <c r="L42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12">
+      <c r="J43" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43">
+        <f>LN(K42/K31)</f>
+        <v>1.195656004953505</v>
+      </c>
+      <c r="L43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12">
+      <c r="J44" t="s">
+        <v>50</v>
+      </c>
+      <c r="K44">
+        <f>K43*K33</f>
+        <v>9.9406840251834404E-3</v>
+      </c>
+      <c r="L44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12">
+      <c r="J45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K45">
+        <f>K44*298</f>
+        <v>2.9623238395046654</v>
+      </c>
+      <c r="L45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12">
+      <c r="J47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K47">
+        <f>K42*0.00000000000001</f>
+        <v>0.20504878277226285</v>
+      </c>
+      <c r="L47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="6:12">
+      <c r="J48" t="s">
+        <v>48</v>
+      </c>
+      <c r="K48">
+        <f>LN(K47/K31)</f>
+        <v>-31.040535296963135</v>
+      </c>
+      <c r="L48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12">
+      <c r="J49" t="s">
+        <v>50</v>
+      </c>
+      <c r="K49">
+        <f>K48*K33</f>
+        <v>-0.25807101045895153</v>
+      </c>
+      <c r="L49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12">
+      <c r="J50" t="s">
+        <v>54</v>
+      </c>
+      <c r="K50">
+        <f>K49*298</f>
+        <v>-76.905161116767559</v>
+      </c>
+      <c r="L50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12">
+      <c r="K51">
+        <f>29.7-K50</f>
+        <v>106.60516111676756</v>
+      </c>
+    </row>
+    <row r="53" spans="10:12">
+      <c r="J53" s="7"/>
+    </row>
+    <row r="54" spans="10:12">
+      <c r="J54" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>